<commit_message>
3 forms work with quote substitution and randomized external IDs
</commit_message>
<xml_diff>
--- a/example-test-forms/DRC USAID Full Census 4.2.xlsx
+++ b/example-test-forms/DRC USAID Full Census 4.2.xlsx
@@ -1295,52 +1295,52 @@
     <t>Is First Visit NAH? - Calculation</t>
   </si>
   <si>
-    <t>tw.drill_down.country.value = "DRC2" ;</t>
+    <t>tw.drill_down.country.value = ”DRC2” ;</t>
   </si>
   <si>
     <t>if ( tw.drill_down.is_available_pulled_down.value == null ) 
-{ tw.drill_down.is_first_visit_calculation.value = "True2" ; }
-else { tw.drill_down.is_first_visit_calculation.value = "False2" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.drill_down.nah_revisit_workflow_pulled_down.value == "true" ) { tw.drill_down.is_nah_revisit_calculation.value = "True2" ; } 
-else { tw.drill_down.is_nah_revisit_calculation.value = "False2" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.drill_down.is_first_visit_calculation.value == "False2" &amp;amp;&amp;amp; tw.drill_down.is_nah_revisit_calculation.value == "False2" ) 
-{ tw.drill_down.is_at_home_revisit_calculation.value = "True2" ; } 
-else { tw.drill_down.is_at_home_revisit_calculation.value = "False2" ; }</t>
+{ tw.drill_down.is_first_visit_calculation.value = ”True2” ; }
+else { tw.drill_down.is_first_visit_calculation.value = ”False2” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.drill_down.nah_revisit_workflow_pulled_down.value == ”true” ) { tw.drill_down.is_nah_revisit_calculation.value = ”True2” ; } 
+else { tw.drill_down.is_nah_revisit_calculation.value = ”False2” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.drill_down.is_first_visit_calculation.value == ”False2” &amp;amp;&amp;amp; tw.drill_down.is_nah_revisit_calculation.value == ”False2” ) 
+{ tw.drill_down.is_at_home_revisit_calculation.value = ”True2” ; } 
+else { tw.drill_down.is_at_home_revisit_calculation.value = ”False2” ; }</t>
   </si>
   <si>
     <t>if ( tw.drill_down.is_available_pulled_down.value === null || tw.drill_down.is_available_pulled_down.value === ’null’ )
-{ tw.drill_down.should_s3_show.value = "True" ; }
-else if ( tw.drill_down.is_18_available_pulled_down.value === null || tw.drill_down.is_18_available_pulled_down.value === ’null’ || tw.drill_down.is_there_someone_else_18_pulled_down.value == "Oui [Ndiyo]") 
-{ tw.drill_down.should_s3_show.value = "True" ; }
-else if ( tw.drill_down.is_family_member_or_renter_pulled_down.value == "Aucune personne présente n’est un membre de la famille ou un locataire [Hakuna memba wa familia au mpagaji hii ao mpangaji katika nyumba hii]" ) 
-{ tw.drill_down.should_s3_show.value = "True" ; }
-else if ( tw.drill_down.nah_revisit_workflow_pulled_down.value == "True" &amp;amp;&amp;amp; tw.drill_down.has_youths_pulled_down.value === null )
-{ tw.drill_down.should_s3_show.value = "True" ; } 
-else {tw.drill_down.should_s3_show.value = "False" ;}</t>
+{ tw.drill_down.should_s3_show.value = ”True” ; }
+else if ( tw.drill_down.is_18_available_pulled_down.value === null || tw.drill_down.is_18_available_pulled_down.value === ’null’ || tw.drill_down.is_there_someone_else_18_pulled_down.value == ”Oui [Ndiyo]”) 
+{ tw.drill_down.should_s3_show.value = ”True” ; }
+else if ( tw.drill_down.is_family_member_or_renter_pulled_down.value == ”Aucune personne présente n’est un membre de la famille ou un locataire [Hakuna memba wa familia au mpagaji hii ao mpangaji katika nyumba hii]” ) 
+{ tw.drill_down.should_s3_show.value = ”True” ; }
+else if ( tw.drill_down.nah_revisit_workflow_pulled_down.value == ”True” &amp;amp;&amp;amp; tw.drill_down.has_youths_pulled_down.value === null )
+{ tw.drill_down.should_s3_show.value = ”True” ; } 
+else {tw.drill_down.should_s3_show.value = ”False” ;}</t>
   </si>
   <si>
     <t>if ( tw.drill_down.is_available_pulled_down.value == null || tw.drill_down.is_18_available_pulled_down.value == null || tw.drill_down.has_youths_pulled_down.value == null) 
-{ tw.drill_down.should_s4_show.value = "True" ; }
-else if ( tw.drill_down.is_nah_revisit_calculation.value == "True2" || tw.drill_down.has_youths_pulled_down.value == "Personne ici présent sait [Hakuna yeyote hapa anajua]" || tw.drill_down.is_there_someone_else_18_pulled_down.value == "Oui [Ndiyo]" )
-{tw.drill_down.should_s4_show.value = "True" ;}
-else {tw.drill_down.should_s4_show.value = "False" ;}</t>
+{ tw.drill_down.should_s4_show.value = ”True” ; }
+else if ( tw.drill_down.is_nah_revisit_calculation.value == ”True2” || tw.drill_down.has_youths_pulled_down.value == ”Personne ici présent sait [Hakuna yeyote hapa anajua]” || tw.drill_down.is_there_someone_else_18_pulled_down.value == ”Oui [Ndiyo]” )
+{tw.drill_down.should_s4_show.value = ”True” ;}
+else {tw.drill_down.should_s4_show.value = ”False” ;}</t>
   </si>
   <si>
     <t>var startTime = new Date() ; if ( tw.drill_down.start_time.value == null || tw.drill_down.start_time.value === ’’ || tw.drill_down.start_time.value == ’null’ ) { tw.drill_down.start_time.value = startTime ; }</t>
   </si>
   <si>
-    <t>var token = " " ; 
+    <t>var token = ” ” ; 
 var dateint = new Date().getTime() ; 
 var datestr = dateint.toString() ; 
 var date = datestr.substring(8) ; 
 var deviceidlong = tw.getIMEI() ; 
 var deviceidstr = deviceidlong.toString() ; 
 var deviceidshort = deviceidstr.substring(13) ; 
-var token = date + "-" + deviceidshort ; 
+var token = date + ”-” + deviceidshort ; 
 if ( tw.drill_down.token_number_pulled_down.value !== null )
 { tw.locating_the_household.token_number.value = tw.drill_down.token_number_pulled_down.value ; }
 else if (tw.locating_the_household.token_number.value == null)
@@ -1351,58 +1351,58 @@
   </si>
   <si>
     <t>var tokenIsBlank = tw.drill_down.token_number_pulled_down.value === null || tw.drill_down.token_number_pulled_down.value === ’’ || tw.drill_down.token_number_pulled_down.value === ’null’ ;
-if ( !tokenIsBlank ) { tw.locating_the_household.needs_token_calculation.value = "False" ; }
-else { tw.locating_the_household.needs_token_calculation.value = "True" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.locating_the_household.is_there_new_info.value == "Non [Hapana]" || tw.locating_the_household.available_yes_no.value == "Non [Hapana]" )
-{ tw.locating_the_household.should_youth_questionnaire_show_pt_2.value = "False" ; }
-else { tw.locating_the_household.should_youth_questionnaire_show_pt_2.value = "True" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.drill_down.is_first_visit_calculation.value == "True2" &amp;amp;&amp;amp; tw.locating_the_household.available_yes_no.value == "Oui [Ndiyo]" ) { tw.locating_the_household.avail_or_new_info.value = "True" ; }
-else if ( tw.drill_down.is_first_visit_calculation.value == "False2" &amp;amp;&amp;amp; tw.locating_the_household.is_there_new_info.value == "Oui [Ndiyo]" ) { tw.locating_the_household.avail_or_new_info.value = "True" ; }
-else { tw.locating_the_household.avail_or_new_info.value = "False" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.drill_down.is_at_home_revisit_calculation.value == "True2" &amp;amp;&amp;amp; tw.locating_the_household.is_there_new_info.value == "Oui [Ndiyo]" ) 
-{ tw.locating_the_household.new_info_at_home.value = "True" ; }
-else { tw.locating_the_household.new_info_at_home.value = "False" ; }</t>
-  </si>
-  <si>
-    <t>if (tw.participation_and_consent.refusing_household_position.value == "Oui [Ndiyo]")
-{ tw.participation_and_consent.family_or_renter_calc.value = "True" ; }
-else {tw.participation_and_consent.family_or_renter_calc.value = "False" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.participation_and_consent.refusing_household_position.value == "Non [Hapana]" ||  tw.participation_and_consent.above_18_other_later_yes_no.value == "Oui [Ndiyo]" )
-{ tw.participation_and_consent.available_first_visit.value = "True" ; }
-else { tw.participation_and_consent.available_first_visit.value = "False" ; }</t>
-  </si>
-  <si>
-    <t>var noReasonProvided = tw.participation_and_consent.revisit_time_multi.value.contains("Je ne sais pas [Sijui]"); 
-var otherReasonProvided = tw.participation_and_consent.revisit_time_multi.value.contains("Matin en semaine [Asubuyi siku la juma]") || tw.participation_and_consent.revisit_time_multi.value.contains("Après-midi en semaine [Kisha mchana siku la juma]") || tw.participation_and_consent.revisit_time_multi.value.contains("Samedi matin [Jumamosi asubuyi]") || tw.participation_and_consent.revisit_time_multi.value.contains("Samedi après-midi [Jumamosi kisha mchana]") || tw.participation_and_consent.revisit_time_multi.value.contains("Dimanche matin [Jumapili asubuyi]") || tw.participation_and_consent.revisit_time_multi.value.contains("Dimanche après-midi [Jumapili kisha mchana]") || tw.participation_and_consent.revisit_time_multi.value.contains("A partir d’une date précise (sélectionner dans la question suivante) [Kwa tarehe ijulikanayo (changua ndani ya swali ifuuatao)]");
-if (noReasonProvided &amp;amp;&amp;amp; otherReasonProvided) { throw "Vous avez sélectionné la réponse Je ne sais pas et une autre reponse! [Ulichagua Sijui na jibu yengine!]"; }</t>
+if ( !tokenIsBlank ) { tw.locating_the_household.needs_token_calculation.value = ”False” ; }
+else { tw.locating_the_household.needs_token_calculation.value = ”True” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.locating_the_household.is_there_new_info.value == ”Non [Hapana]” || tw.locating_the_household.available_yes_no.value == ”Non [Hapana]” )
+{ tw.locating_the_household.should_youth_questionnaire_show_pt_2.value = ”False” ; }
+else { tw.locating_the_household.should_youth_questionnaire_show_pt_2.value = ”True” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.drill_down.is_first_visit_calculation.value == ”True2” &amp;amp;&amp;amp; tw.locating_the_household.available_yes_no.value == ”Oui [Ndiyo]” ) { tw.locating_the_household.avail_or_new_info.value = ”True” ; }
+else if ( tw.drill_down.is_first_visit_calculation.value == ”False2” &amp;amp;&amp;amp; tw.locating_the_household.is_there_new_info.value == ”Oui [Ndiyo]” ) { tw.locating_the_household.avail_or_new_info.value = ”True” ; }
+else { tw.locating_the_household.avail_or_new_info.value = ”False” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.drill_down.is_at_home_revisit_calculation.value == ”True2” &amp;amp;&amp;amp; tw.locating_the_household.is_there_new_info.value == ”Oui [Ndiyo]” ) 
+{ tw.locating_the_household.new_info_at_home.value = ”True” ; }
+else { tw.locating_the_household.new_info_at_home.value = ”False” ; }</t>
+  </si>
+  <si>
+    <t>if (tw.participation_and_consent.refusing_household_position.value == ”Oui [Ndiyo]”)
+{ tw.participation_and_consent.family_or_renter_calc.value = ”True” ; }
+else {tw.participation_and_consent.family_or_renter_calc.value = ”False” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.participation_and_consent.refusing_household_position.value == ”Non [Hapana]” ||  tw.participation_and_consent.above_18_other_later_yes_no.value == ”Oui [Ndiyo]” )
+{ tw.participation_and_consent.available_first_visit.value = ”True” ; }
+else { tw.participation_and_consent.available_first_visit.value = ”False” ; }</t>
+  </si>
+  <si>
+    <t>var noReasonProvided = tw.participation_and_consent.revisit_time_multi.value.contains(”Je ne sais pas [Sijui]”); 
+var otherReasonProvided = tw.participation_and_consent.revisit_time_multi.value.contains(”Matin en semaine [Asubuyi siku la juma]”) || tw.participation_and_consent.revisit_time_multi.value.contains(”Après-midi en semaine [Kisha mchana siku la juma]”) || tw.participation_and_consent.revisit_time_multi.value.contains(”Samedi matin [Jumamosi asubuyi]”) || tw.participation_and_consent.revisit_time_multi.value.contains(”Samedi après-midi [Jumamosi kisha mchana]”) || tw.participation_and_consent.revisit_time_multi.value.contains(”Dimanche matin [Jumapili asubuyi]”) || tw.participation_and_consent.revisit_time_multi.value.contains(”Dimanche après-midi [Jumapili kisha mchana]”) || tw.participation_and_consent.revisit_time_multi.value.contains(”A partir d’une date précise (sélectionner dans la question suivante) [Kwa tarehe ijulikanayo (changua ndani ya swali ifuuatao)]”);
+if (noReasonProvided &amp;amp;&amp;amp; otherReasonProvided) { throw ”Vous avez sélectionné la réponse Je ne sais pas et une autre reponse! [Ulichagua Sijui na jibu yengine!]”; }</t>
   </si>
   <si>
     <t>var dt = tw.participation_and_consent.revisit_when.value ; 
-if (dt.getFullYear() &amp;lt;=2018) {throw "Le moment de la visite suivante ne peut pas être dans le passé! [Wakati wa kurudi hauwezi kuwa kwa muda iliyo pita!]" ;}
-else if (dt.getFullYear() == 2019 &amp;amp;&amp;amp; dt.getMonth() &amp;lt;7) {throw "Le moment de la visite suivante ne peut pas être dans le passé! [Wakati wa kurudi hauwezi kuwa kwa muda iliyo pita!]" ;}</t>
-  </si>
-  <si>
-    <t>if (tw.hh_presence.youth_amt.value &amp;gt;=8) {throw "Cet enquête permet d’avoir un maximum de 7 jeunes. Veuillez entrer 7, même s’il y a plus de 7 jeunes dans ce ménage. [Utafiti huu huruhusu vijana 7 upeo. Tafadhali ingiza 7, hata ikiwa kuna vijana zaidi ya vijana katika kaya hii.]" ;}
-else if (tw.hh_presence.youth_amt.value &amp;lt; 1) {throw "Vous ne pouvez pas entrer 0 parce que vous avez indiqué qu’il y a des jeunes dans ce ménage! [Haiwezi kuwa na vijana zaidi ya kusema sasa kuliko kuna vijana katika nyumba!]" ;}</t>
+if (dt.getFullYear() &amp;lt;=2018) {throw ”Le moment de la visite suivante ne peut pas être dans le passé! [Wakati wa kurudi hauwezi kuwa kwa muda iliyo pita!]” ;}
+else if (dt.getFullYear() == 2019 &amp;amp;&amp;amp; dt.getMonth() &amp;lt;7) {throw ”Le moment de la visite suivante ne peut pas être dans le passé! [Wakati wa kurudi hauwezi kuwa kwa muda iliyo pita!]” ;}</t>
+  </si>
+  <si>
+    <t>if (tw.hh_presence.youth_amt.value &amp;gt;=8) {throw ”Cet enquête permet d’avoir un maximum de 7 jeunes. Veuillez entrer 7, même s’il y a plus de 7 jeunes dans ce ménage. [Utafiti huu huruhusu vijana 7 upeo. Tafadhali ingiza 7, hata ikiwa kuna vijana zaidi ya vijana katika kaya hii.]” ;}
+else if (tw.hh_presence.youth_amt.value &amp;lt; 1) {throw ”Vous ne pouvez pas entrer 0 parce que vous avez indiqué qu’il y a des jeunes dans ce ménage! [Haiwezi kuwa na vijana zaidi ya kusema sasa kuliko kuna vijana katika nyumba!]” ;}</t>
   </si>
   <si>
     <t>var tendigitRegex = /^0[8,9]{1}\d{8}$/ ; 
-if (!tendigitRegex.test(tw.hh_presence.resp_phone_num.value)) {throw "Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya ku achanisha, au herufi nyingine maalum.]" ; }</t>
+if (!tendigitRegex.test(tw.hh_presence.resp_phone_num.value)) {throw ”Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya ku achanisha, au herufi nyingine maalum.]” ; }</t>
   </si>
   <si>
     <t>var tendigitRegex = /^0[8,9]{1}\d{8}$/ ; 
 if (!tendigitRegex.test(tw.hh_presence.resp_phone_num_2.value)) 
-{throw "Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya ku achanisha, au herufi nyingine maalum.]" ; }
+{throw ”Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya ku achanisha, au herufi nyingine maalum.]” ; }
 else if (tw.hh_presence.resp_phone_num_2.value == tw.hh_presence.resp_phone_num.value) 
-{throw "Ce téléphone doit être différent du numéro de téléphone principal! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako!]" ; }</t>
+{throw ”Ce téléphone doit être différent du numéro de téléphone principal! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako!]” ; }</t>
   </si>
   <si>
     <t>var numIsBlank = tw.drill_down.number_of_youths_to_revisit_pulled_down.value === ’’ || tw.drill_down.number_of_youths_to_revisit_pulled_down.value  === null || tw.drill_down.number_of_youths_to_revisit_pulled_down.value === ’null’ ;
@@ -1410,178 +1410,178 @@
 else { tw.calculating_youths.youths_not_in_census_calculation.value = parseInt( tw.hh_presence.youth_amt.value ) ; }</t>
   </si>
   <si>
-    <t>var indInfoString = "Il y a " + tw.calculating_youths.youths_not_in_census_calculation.value + " jeune(s) au total dans ce ménage à enquêter maintenant. Cette section va se repéter " + tw.calculating_youths.youths_not_in_census_calculation.value + " fois. [Wapo vijana " + tw.calculating_youths.youths_not_in_census_calculation.value + " katika nyumba hii. Hii sehemu ya utafiti ita rudiya mara " + tw.calculating_youths.youths_not_in_census_calculation.value + ".]" ; 
+    <t>var indInfoString = ”Il y a ” + tw.calculating_youths.youths_not_in_census_calculation.value + ” jeune(s) au total dans ce ménage à enquêter maintenant. Cette section va se repéter ” + tw.calculating_youths.youths_not_in_census_calculation.value + ” fois. [Wapo vijana ” + tw.calculating_youths.youths_not_in_census_calculation.value + ” katika nyumba hii. Hii sehemu ya utafiti ita rudiya mara ” + tw.calculating_youths.youths_not_in_census_calculation.value + ”.]” ; 
 tw.youth_data.current.fo_youth_summary.value = indInfoString ;</t>
   </si>
   <si>
-    <t>if ( tw.youth_data.current.name_pulled_down.value == "Unknown" ) { tw.youth_data.current.is_name_unknown_calculation.value = "True" ; }
-else { tw.youth_data.current.is_name_unknown_calculation.value = "False" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.name_pulled_down.value !== null &amp;amp;&amp;amp; tw.youth_data.current.name_pulled_down.value !== "Unknown" ) 
-{ tw.youth_data.current.is_name_real_name_calculation.value = "True" ; }
-else { tw.youth_data.current.is_name_real_name_calculation.value = "False" ; }</t>
-  </si>
-  <si>
-    <t>var indInfoString = "Pour cette section, veuillez recueillir des renseignements sur le jeune avec le nom " + tw.youth_data.current.name_pulled_down.value + "." ;
+    <t>if ( tw.youth_data.current.name_pulled_down.value == ”Unknown” ) { tw.youth_data.current.is_name_unknown_calculation.value = ”True” ; }
+else { tw.youth_data.current.is_name_unknown_calculation.value = ”False” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.name_pulled_down.value !== null &amp;amp;&amp;amp; tw.youth_data.current.name_pulled_down.value !== ”Unknown” ) 
+{ tw.youth_data.current.is_name_real_name_calculation.value = ”True” ; }
+else { tw.youth_data.current.is_name_real_name_calculation.value = ”False” ; }</t>
+  </si>
+  <si>
+    <t>var indInfoString = ”Pour cette section, veuillez recueillir des renseignements sur le jeune avec le nom ” + tw.youth_data.current.name_pulled_down.value + ”.” ;
 tw.youth_data.current.show_youth_name.value = indInfoString ;</t>
   </si>
   <si>
-    <t>if ( ( tw.youth_data.current.youth_carte_yes_no.value == "Oui, pas vu [Ndio, haionekane]" || tw.youth_data.current.has_youths_carte.value == "Oui, mais le document n’est pas present [Ndio, kadi haionekani kwa sasa]" ) &amp;amp;&amp;amp; ( tw.youth_data.current.no_carte_picklist.value == "La carte a été perdue [Ilipotea]" || tw.youth_data.current.no_carte_picklist.value == "La carte a été volée [Ili ibwa]" || tw.youth_data.current.no_carte_picklist.value == "La carte a été détruit (incendie, lave-linge, etc.) [Isha haribishwa (moto, maji, etc.)]") ) 
-{ throw "Si la carte est perdue, volée, ou détruit, veuillez retourner à la question précédente et sélectionner ’Non’. [Kama kadi ilipotea ao ilibiwa, tafadhali rudi uchaguwe ’Hapana’ kwa swali ya nyuma.]" ; } 
-else if ( ( tw.youth_data.current.youth_carte_yes_no.value == "Non [Hapana]" || tw.youth_data.current.has_youths_carte.value == "Non, le jeune ne possède pas une carte d’electeur [Hapana, kijana hana kadi ya kura]" ) &amp;amp;&amp;amp; ( tw.youth_data.current.no_carte_picklist.value == "La carte est enfermée dans une autre chambre par les parents / conjoint / autre [Kadi iko katika chumba ya kufungiwa na wazazi / bibi ao bwana / mwengine]" || tw.youth_data.current.no_carte_picklist.value == "La carte est dans la maison, mais ne peut pas être trouvée en ce moment [Kadi iko katika nyumba, alakini sijue wapi kwa saha hii]" || tw.youth_data.current.no_carte_picklist.value == "La carte est retenue par le parent / conjoint / autre qui n’est pas présent [Mzazi / bibi ao bwana / mwengine njo iko na kadi yangu]" || tw.youth_data.current.no_carte_picklist.value == "La carte a été laissée à un ami ou à un membre de la famille, mais peut être récupérée [Kadi iliachiwa kwa rafiki ao mtu wa familiya, ina weza patikana]" || tw.youth_data.current.no_carte_picklist.value == "La carte est conservée au lieu de travail / l’école du jeune [Kadi iko kwenye fasi y’a Kazi / masomo ya kijana]" ) ) 
-{ throw "Si le jeune n’a pas de carte, vous ne pouvez pas choisir cette raison. [ SWAHILI ]" ; }</t>
+    <t>if ( ( tw.youth_data.current.youth_carte_yes_no.value == ”Oui, pas vu [Ndio, haionekane]” || tw.youth_data.current.has_youths_carte.value == ”Oui, mais le document n’est pas present [Ndio, kadi haionekani kwa sasa]” ) &amp;amp;&amp;amp; ( tw.youth_data.current.no_carte_picklist.value == ”La carte a été perdue [Ilipotea]” || tw.youth_data.current.no_carte_picklist.value == ”La carte a été volée [Ili ibwa]” || tw.youth_data.current.no_carte_picklist.value == ”La carte a été détruit (incendie, lave-linge, etc.) [Isha haribishwa (moto, maji, etc.)]”) ) 
+{ throw ”Si la carte est perdue, volée, ou détruit, veuillez retourner à la question précédente et sélectionner ’Non’. [Kama kadi ilipotea ao ilibiwa, tafadhali rudi uchaguwe ’Hapana’ kwa swali ya nyuma.]” ; } 
+else if ( ( tw.youth_data.current.youth_carte_yes_no.value == ”Non [Hapana]” || tw.youth_data.current.has_youths_carte.value == ”Non, le jeune ne possède pas une carte d’electeur [Hapana, kijana hana kadi ya kura]” ) &amp;amp;&amp;amp; ( tw.youth_data.current.no_carte_picklist.value == ”La carte est enfermée dans une autre chambre par les parents / conjoint / autre [Kadi iko katika chumba ya kufungiwa na wazazi / bibi ao bwana / mwengine]” || tw.youth_data.current.no_carte_picklist.value == ”La carte est dans la maison, mais ne peut pas être trouvée en ce moment [Kadi iko katika nyumba, alakini sijue wapi kwa saha hii]” || tw.youth_data.current.no_carte_picklist.value == ”La carte est retenue par le parent / conjoint / autre qui n’est pas présent [Mzazi / bibi ao bwana / mwengine njo iko na kadi yangu]” || tw.youth_data.current.no_carte_picklist.value == ”La carte a été laissée à un ami ou à un membre de la famille, mais peut être récupérée [Kadi iliachiwa kwa rafiki ao mtu wa familiya, ina weza patikana]” || tw.youth_data.current.no_carte_picklist.value == ”La carte est conservée au lieu de travail / l’école du jeune [Kadi iko kwenye fasi y’a Kazi / masomo ya kijana]” ) ) 
+{ throw ”Si le jeune n’a pas de carte, vous ne pouvez pas choisir cette raison. [ SWAHILI ]” ; }</t>
   </si>
   <si>
     <t>var str = tw.youth_data.current.youth_carte_no_reason.value ; 
 var length = str.length ; 
-if (length &amp;lt; 20) {throw "Minimum 20 caractères. Veuillez entrer plus d’informations pour cette description. [Kiwango cha chini cha herufi 20. Tafadhali ingiza zaidi kwa maelezo haya.]" ;}</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.youth_carte_yes_no.value == "Oui, l’original ou photocopie [Ndio, kadi orijinal au fotocopi ipo]" || tw.youth_data.current.youth_carte_yes_no.value == "Oui, pas vu [Ndio, haionekane]" || tw.youth_data.current.has_youths_carte.value == "Oui, et le document est present [Ndio kadi ipo]" || tw.youth_data.current.has_youths_carte.value == "Oui, mais le document n’est pas present [Ndio, kadi haionekani kwa sasa]" )
-{ tw.youth_data.current.has_carte_delecteur_yes_no.value = "True2" ; }
-else { tw.youth_data.current.has_carte_delecteur_yes_no.value = "False2" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.has_carte_delecteur_yes_no.value == "False2" ) { tw.youth_data.current.has_no_id_documents_calculation.value = "True2" ;}
-else { tw.youth_data.current.has_no_id_documents_calculation.value = "False2" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.youth_carte_yes_no.value == "Oui, l’original ou photocopie [Ndio, kadi orijinal au fotocopi ipo]" || tw.youth_data.current.has_youths_carte.value == "Oui, et le document est present [Ndio kadi ipo]" ) { tw.youth_data.current.has_carte_delecteur_present_calculation.value = "True" ; } else { tw.youth_data.current.has_carte_delecteur_present_calculation.value = "False" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.confirm_nah_and_no_docs.value == "Non [Hapana]" ) { throw "Veuillez retourner en arriére dans le sondage pour remplir les renseignements sur les jeunes. [Tafadhali, rudi nyuma katika maulizo, nauulize swali kuhusu vijana.]" ;}</t>
-  </si>
-  <si>
-    <t>if(tw.youth_data.current.youth_name_carte_reentry.value !== tw.youth_data.current.youth_name_carte.value) {throw "Ce nom ne correspond pas au nom que vous venez d’entrer! [Jina hili halihusiani na jina uliloingiza sasa hivi!]" ; }</t>
+if (length &amp;lt; 20) {throw ”Minimum 20 caractères. Veuillez entrer plus d’informations pour cette description. [Kiwango cha chini cha herufi 20. Tafadhali ingiza zaidi kwa maelezo haya.]” ;}</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.youth_carte_yes_no.value == ”Oui, l’original ou photocopie [Ndio, kadi orijinal au fotocopi ipo]” || tw.youth_data.current.youth_carte_yes_no.value == ”Oui, pas vu [Ndio, haionekane]” || tw.youth_data.current.has_youths_carte.value == ”Oui, et le document est present [Ndio kadi ipo]” || tw.youth_data.current.has_youths_carte.value == ”Oui, mais le document n’est pas present [Ndio, kadi haionekani kwa sasa]” )
+{ tw.youth_data.current.has_carte_delecteur_yes_no.value = ”True2” ; }
+else { tw.youth_data.current.has_carte_delecteur_yes_no.value = ”False2” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.has_carte_delecteur_yes_no.value == ”False2” ) { tw.youth_data.current.has_no_id_documents_calculation.value = ”True2” ;}
+else { tw.youth_data.current.has_no_id_documents_calculation.value = ”False2” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.youth_carte_yes_no.value == ”Oui, l’original ou photocopie [Ndio, kadi orijinal au fotocopi ipo]” || tw.youth_data.current.has_youths_carte.value == ”Oui, et le document est present [Ndio kadi ipo]” ) { tw.youth_data.current.has_carte_delecteur_present_calculation.value = ”True” ; } else { tw.youth_data.current.has_carte_delecteur_present_calculation.value = ”False” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.confirm_nah_and_no_docs.value == ”Non [Hapana]” ) { throw ”Veuillez retourner en arriére dans le sondage pour remplir les renseignements sur les jeunes. [Tafadhali, rudi nyuma katika maulizo, nauulize swali kuhusu vijana.]” ;}</t>
+  </si>
+  <si>
+    <t>if(tw.youth_data.current.youth_name_carte_reentry.value !== tw.youth_data.current.youth_name_carte.value) {throw ”Ce nom ne correspond pas au nom que vous venez d’entrer! [Jina hili halihusiani na jina uliloingiza sasa hivi!]” ; }</t>
   </si>
   <si>
     <t>var d1 = new Date(tw.youth_data.current.carte_dob_reentry.value) ; 
 var d2 = new Date(tw.youth_data.current.carte_dob.value) ; 
-if ( d1.getFullYear() !== d2.getFullYear() ) {throw "Cette année ne correspond pas à l’année que vous avez sasie! [Mwaka huu sio sawa na mwaka ambao ume ingiza sasa hivi!]" ;}
-else if ( d1.getMonth() !== d2.getMonth() ) {throw "Ce mois ne correspond pas au mois que vous avez saisie! [Mwezi huu hailingani na mwezi ulioingiza sasa hivi!]" ;}
-else if ( d1.getDate() !== d2.getDate() ) {throw "Cette date ne correspond pas à la date que vous avez saisie! [Tarehe hii hailingani na tarehe ambayo umeingiza sasa hivi!]" ;}</t>
+if ( d1.getFullYear() !== d2.getFullYear() ) {throw ”Cette année ne correspond pas à l’année que vous avez sasie! [Mwaka huu sio sawa na mwaka ambao ume ingiza sasa hivi!]” ;}
+else if ( d1.getMonth() !== d2.getMonth() ) {throw ”Ce mois ne correspond pas au mois que vous avez saisie! [Mwezi huu hailingani na mwezi ulioingiza sasa hivi!]” ;}
+else if ( d1.getDate() !== d2.getDate() ) {throw ”Cette date ne correspond pas à la date que vous avez saisie! [Tarehe hii hailingani na tarehe ambayo umeingiza sasa hivi!]” ;}</t>
   </si>
   <si>
     <t>var tendigitRegex = /^\d{11}$/ ; 
-if (!tendigitRegex.test(tw.youth_data.current.carte_num.value)) {throw "La carte d’électeur devrait contenir 11 chiffres sans tirets, espaces, ou autres caractères spéciaux. [Nambari ya kadi ya uchaguzi inapashwa kuwa na namba 11 bila nukta, nafasi ya kuunganisha maneno (espace), ao zengine miandiko za ki pekee.]" ; }</t>
-  </si>
-  <si>
-    <t>if(tw.youth_data.current.carte_num_reentry.value !== tw.youth_data.current.carte_num.value) {throw "Ce numéro ne correspond pas à celui que vous venez d’entrer! [Nambari hii hailingani na nambari uliyoingia hivi karibuni!]" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.youth_name_from_youth_reentry.value !== tw.youth_data.current.youth_name_from_youth.value ) { throw "Ce nom ne correspond pas au nom que vous venez d’entrer! [Jina hili halihusiani na jina uliloingiza sasa hivi!]" ; }</t>
+if (!tendigitRegex.test(tw.youth_data.current.carte_num.value)) {throw ”La carte d’électeur devrait contenir 11 chiffres sans tirets, espaces, ou autres caractères spéciaux. [Nambari ya kadi ya uchaguzi inapashwa kuwa na namba 11 bila nukta, nafasi ya kuunganisha maneno (espace), ao zengine miandiko za ki pekee.]” ; }</t>
+  </si>
+  <si>
+    <t>if(tw.youth_data.current.carte_num_reentry.value !== tw.youth_data.current.carte_num.value) {throw ”Ce numéro ne correspond pas à celui que vous venez d’entrer! [Nambari hii hailingani na nambari uliyoingia hivi karibuni!]” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.youth_name_from_youth_reentry.value !== tw.youth_data.current.youth_name_from_youth.value ) { throw ”Ce nom ne correspond pas au nom que vous venez d’entrer! [Jina hili halihusiani na jina uliloingiza sasa hivi!]” ; }</t>
   </si>
   <si>
     <t>var d1 = new Date(tw.youth_data.current.dob_no_doc_reentry.value) ; 
 var d2 = new Date(tw.youth_data.current.dob_no_doc.value) ; 
-if ( d1.getFullYear() !== d2.getFullYear() ) {throw "Cette année ne correspond pas à l’année que vous avez saisie! [Mwaka huu sio sawa na mwaka ambao ume ingiza sasa hivi!]" ;}
-else if ( d1.getMonth() !== d2.getMonth() ) {throw "Ce mois ne correspond pas au mois que vous avez saisie! [Mwezi huu hailingani na mwezi ulioingiza sasa hivi!]" ;}
-else if ( d1.getDate() !== d2.getDate() ) {throw "Cette date ne correspond pas à la date que vous avez saisie! [Tarehe hii hailingani na tarehe ambayo umeingiza sasa hivi!]" ;}</t>
+if ( d1.getFullYear() !== d2.getFullYear() ) {throw ”Cette année ne correspond pas à l’année que vous avez saisie! [Mwaka huu sio sawa na mwaka ambao ume ingiza sasa hivi!]” ;}
+else if ( d1.getMonth() !== d2.getMonth() ) {throw ”Ce mois ne correspond pas au mois que vous avez saisie! [Mwezi huu hailingani na mwezi ulioingiza sasa hivi!]” ;}
+else if ( d1.getDate() !== d2.getDate() ) {throw ”Cette date ne correspond pas à la date que vous avez saisie! [Tarehe hii hailingani na tarehe ambayo umeingiza sasa hivi!]” ;}</t>
   </si>
   <si>
     <t>var tendigitRegex = /^0[8,9]{1}\d{8}$/ ; 
-if (!tendigitRegex.test(tw.youth_data.current.phone_number_one.value)) {throw "Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya ku achanisha, au herufi nyingine maalum.]" ; }</t>
-  </si>
-  <si>
-    <t>if(tw.youth_data.current.phone_number_one_reentry.value != tw.youth_data.current.phone_number_one.value) {throw "Ce numéro de téléphone ne correspond pas à celui que vous venez d’entrer! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]" ; }</t>
+if (!tendigitRegex.test(tw.youth_data.current.phone_number_one.value)) {throw ”Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya ku achanisha, au herufi nyingine maalum.]” ; }</t>
+  </si>
+  <si>
+    <t>if(tw.youth_data.current.phone_number_one_reentry.value != tw.youth_data.current.phone_number_one.value) {throw ”Ce numéro de téléphone ne correspond pas à celui que vous venez d’entrer! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]” ; }</t>
   </si>
   <si>
     <t>var tendigitRegex = /^0[8,9]{1}\d{8}$/ ; 
-if (!tendigitRegex.test(tw.youth_data.current.phone_number_two.value)) {throw "Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya ku achanisha, au herufi nyingine maalum.]" ; }
-else if (tw.youth_data.current.phone_number_two.value == tw.youth_data.current.phone_number_one.value) {throw "Ce téléphone doit être différent du numéro de téléphone principal! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]" ;}</t>
-  </si>
-  <si>
-    <t>if(tw.youth_data.current.phone_number_two_reentry.value != tw.youth_data.current.phone_number_two.value) {throw "Ce numéro de téléphone ne correspond pas à celui que vous venez d’entrer! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]" ; }</t>
+if (!tendigitRegex.test(tw.youth_data.current.phone_number_two.value)) {throw ”Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya ku achanisha, au herufi nyingine maalum.]” ; }
+else if (tw.youth_data.current.phone_number_two.value == tw.youth_data.current.phone_number_one.value) {throw ”Ce téléphone doit être différent du numéro de téléphone principal! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]” ;}</t>
+  </si>
+  <si>
+    <t>if(tw.youth_data.current.phone_number_two_reentry.value != tw.youth_data.current.phone_number_two.value) {throw ”Ce numéro de téléphone ne correspond pas à celui que vous venez d’entrer! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]” ; }</t>
   </si>
   <si>
     <t>var tendigitRegex = /^\d{10}$/ ; 
-if (!tendigitRegex.test(tw.youth_data.current.phone_number_three.value)) {throw "Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya kuachanisha, nafasi, au herufi nyingine maalum.]" ; }
-else if (tw.youth_data.current.phone_number_three.value == tw.youth_data.current.phone_number_one.value) {throw "Ce téléphone doit être différent du numéro de téléphone principal! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]" ;}
-else if (tw.youth_data.current.phone_number_three.value == tw.youth_data.current.phone_number_two.value) {throw "Ce numéro de téléphone doit être différent du deuxième numéro de téléphone! [.............]" ;}</t>
-  </si>
-  <si>
-    <t>if(tw.youth_data.current.phone_number_three_entry.value != tw.youth_data.current.phone_number_three.value) {throw "Ce numéro de téléphone ne correspond pas à celui que vous venez d’entrer! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]" ; }</t>
+if (!tendigitRegex.test(tw.youth_data.current.phone_number_three.value)) {throw ”Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya kuachanisha, nafasi, au herufi nyingine maalum.]” ; }
+else if (tw.youth_data.current.phone_number_three.value == tw.youth_data.current.phone_number_one.value) {throw ”Ce téléphone doit être différent du numéro de téléphone principal! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]” ;}
+else if (tw.youth_data.current.phone_number_three.value == tw.youth_data.current.phone_number_two.value) {throw ”Ce numéro de téléphone doit être différent du deuxième numéro de téléphone! [.............]” ;}</t>
+  </si>
+  <si>
+    <t>if(tw.youth_data.current.phone_number_three_entry.value != tw.youth_data.current.phone_number_three.value) {throw ”Ce numéro de téléphone ne correspond pas à celui que vous venez d’entrer! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]” ; }</t>
   </si>
   <si>
     <t>var tendigitRegex =  /^0[8,9]{1}\d{8}$/ ;
-if (!tendigitRegex.test(tw.youth_data.current.not_home_phone_num.value)) {throw "Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya ku achanisha, au herufi nyingine maalum.]" ; }</t>
+if (!tendigitRegex.test(tw.youth_data.current.not_home_phone_num.value)) {throw ”Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya ku achanisha, au herufi nyingine maalum.]” ; }</t>
   </si>
   <si>
     <t>if(tw.youth_data.current.not_home_phone_num_reentry.value != tw.youth_data.current.not_home_phone_num.value) 
-{throw "Ce numéro de téléphone ne correspond pas à celui que vous venez d’entrer! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]" ; }</t>
+{throw ”Ce numéro de téléphone ne correspond pas à celui que vous venez d’entrer! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]” ; }</t>
   </si>
   <si>
     <t>var tendigitRegex = /^0[8,9]{1}\d{8}$/  ;
-if (!tendigitRegex.test(tw.youth_data.current.not_home_phone_sec.value)) {throw "Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya ku achanisha, au herufi nyingine maalum.]" ; }
-else if (tw.youth_data.current.not_home_phone_sec.value == tw.youth_data.current.not_home_phone_num.value) {throw "Ce téléphone doit être différent du numéro de téléphone principal! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]" ;}</t>
+if (!tendigitRegex.test(tw.youth_data.current.not_home_phone_sec.value)) {throw ”Le numéro de téléphone doit commencer par 08 ou 09 et être composé de 10 chiffres sans tirets, espaces ou autres caractères spéciaux. [Nambari ya simu inapaswa kuanza na 08 au 09 na kuwa na nambari 10 bila nukta, nafasi ya ku achanisha, au herufi nyingine maalum.]” ; }
+else if (tw.youth_data.current.not_home_phone_sec.value == tw.youth_data.current.not_home_phone_num.value) {throw ”Ce téléphone doit être différent du numéro de téléphone principal! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]” ;}</t>
   </si>
   <si>
     <t>if(tw.youth_data.current.not_home_phone_sec_reentry.value != tw.youth_data.current.not_home_phone_sec.value) 
-{throw "Ce numéro de téléphone ne correspond pas à celui que vous venez d’entrer! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.twin_yes_no.value == "Oui [Ndiyo]" || tw.youth_data.current.twin_yes_no_2.value == "Oui [Ndiyo]" ) { tw.youth_data.current.twin_status_calculation.value = "Oui [Ndiyo]" ; }
-else { tw.youth_data.current.twin_status_calculation.value = "Non [Hapana]" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.first_born_yes_no.value == "Oui [Ndiyo]" || tw.youth_data.current.first_born_yes_no_2.value == "Oui [Ndiyo]" ) { tw.youth_data.current.first_born_status_calculation.value = "Oui [Ndiyo]" ; }
-else { tw.youth_data.current.first_born_status_calculation.value = "Non [Hapana]" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.has_youths_carte.value == "Oui, et le document est present [Ndio kadi ipo]" || tw.youth_data.current.youth_carte_yes_no.value == "Oui, l’original ou photocopie [Ndio, kadi orijinal au fotocopi ipo]" || tw.youth_data.current.youth_carte_yes_no.value == "Oui, pas vu [Ndio, haionekane]" || tw.youth_data.current.in_person_yes_no.value == "Oui [Ndiyo]" )
-{ tw.youth_data.current.youth_present_or_in_docs.value = "True2" ; }
-else { tw.youth_data.current.youth_present_or_in_docs.value = "False2" ; }</t>
-  </si>
-  <si>
-    <t>tw.youth_data.current.name_verification_status.value = "No Name Mapping Found2";</t>
-  </si>
-  <si>
-    <t>tw.youth_data.current.sanctions_list_status.value = "Unscreened2";</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.name_pulled_down.value !== null &amp;amp;&amp;amp; tw.youth_data.current.name_pulled_down.value !== "Unknown"  &amp;amp;&amp;amp; tw.youth_data.current.has_youths_carte.value == "Oui, et le document est present [Ndio kadi ipo]" ) 
+{throw ”Ce numéro de téléphone ne correspond pas à celui que vous venez d’entrer! [Tafadhali ingiza tena namba ya pili ya simu ya mwongozi wako.]” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.twin_yes_no.value == ”Oui [Ndiyo]” || tw.youth_data.current.twin_yes_no_2.value == ”Oui [Ndiyo]” ) { tw.youth_data.current.twin_status_calculation.value = ”Oui [Ndiyo]” ; }
+else { tw.youth_data.current.twin_status_calculation.value = ”Non [Hapana]” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.first_born_yes_no.value == ”Oui [Ndiyo]” || tw.youth_data.current.first_born_yes_no_2.value == ”Oui [Ndiyo]” ) { tw.youth_data.current.first_born_status_calculation.value = ”Oui [Ndiyo]” ; }
+else { tw.youth_data.current.first_born_status_calculation.value = ”Non [Hapana]” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.has_youths_carte.value == ”Oui, et le document est present [Ndio kadi ipo]” || tw.youth_data.current.youth_carte_yes_no.value == ”Oui, l’original ou photocopie [Ndio, kadi orijinal au fotocopi ipo]” || tw.youth_data.current.youth_carte_yes_no.value == ”Oui, pas vu [Ndio, haionekane]” || tw.youth_data.current.in_person_yes_no.value == ”Oui [Ndiyo]” )
+{ tw.youth_data.current.youth_present_or_in_docs.value = ”True2” ; }
+else { tw.youth_data.current.youth_present_or_in_docs.value = ”False2” ; }</t>
+  </si>
+  <si>
+    <t>tw.youth_data.current.name_verification_status.value = ”No Name Mapping Found2”;</t>
+  </si>
+  <si>
+    <t>tw.youth_data.current.sanctions_list_status.value = ”Unscreened2”;</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.name_pulled_down.value !== null &amp;amp;&amp;amp; tw.youth_data.current.name_pulled_down.value !== ”Unknown”  &amp;amp;&amp;amp; tw.youth_data.current.has_youths_carte.value == ”Oui, et le document est present [Ndio kadi ipo]” ) 
 { tw.youth_data.current.last_name.value = tw.youth_data.current.youth_name_carte.value ; }
-else if ( tw.youth_data.current.name_pulled_down.value !== null &amp;amp;&amp;amp; tw.youth_data.current.name_pulled_down.value !== "Unknown" &amp;amp;&amp;amp; tw.youth_data.current.youth_carte_yes_no.value == "Oui, l’original ou photocopie [Ndio, kadi orijinal au fotocopi ipo]" ) 
+else if ( tw.youth_data.current.name_pulled_down.value !== null &amp;amp;&amp;amp; tw.youth_data.current.name_pulled_down.value !== ”Unknown” &amp;amp;&amp;amp; tw.youth_data.current.youth_carte_yes_no.value == ”Oui, l’original ou photocopie [Ndio, kadi orijinal au fotocopi ipo]” ) 
 { tw.youth_data.current.last_name.value = tw.youth_data.current.youth_name_carte.value ; }
-else if ( tw.youth_data.current.name_pulled_down.value !== null &amp;amp;&amp;amp; tw.youth_data.current.name_pulled_down.value !== "Unknown" ) 
+else if ( tw.youth_data.current.name_pulled_down.value !== null &amp;amp;&amp;amp; tw.youth_data.current.name_pulled_down.value !== ”Unknown” ) 
 { tw.youth_data.current.last_name.value = tw.youth_data.current.name_pulled_down.value ; }
-else if (tw.youth_data.current.has_carte_delecteur_present_calculation.value == "True")
+else if (tw.youth_data.current.has_carte_delecteur_present_calculation.value == ”True”)
 { tw.youth_data.current.last_name.value = tw.youth_data.current.youth_name_carte.value ; }
-else if ( tw.youth_data.current.youth_carte_yes_no.value == "Oui, pas vu [Ndio, haionekane]" )
+else if ( tw.youth_data.current.youth_carte_yes_no.value == ”Oui, pas vu [Ndio, haionekane]” )
 { tw.youth_data.current.last_name.value = tw.youth_data.current.youth_name_from_youth.value ; }
-else if ( tw.youth_data.current.has_youths_carte.value == "Oui, mais le document n’est pas present [Ndio, kadi haionekani kwa sasa]"  || tw.youth_data.current.youth_carte_yes_no.value == "Non [Hapana]"|| tw.youth_data.current.has_youths_carte.value == "Non, le jeune ne possède pas une carte d’electeur [Hapana, kijana hana kadi ya kura]" )
+else if ( tw.youth_data.current.has_youths_carte.value == ”Oui, mais le document n’est pas present [Ndio, kadi haionekani kwa sasa]”  || tw.youth_data.current.youth_carte_yes_no.value == ”Non [Hapana]”|| tw.youth_data.current.has_youths_carte.value == ”Non, le jeune ne possède pas une carte d’electeur [Hapana, kijana hana kadi ya kura]” )
 { tw.youth_data.current.last_name.value = tw.youth_data.current.youth_name_from_youth.value ; }
-else if ( tw.youth_data.current.youth_consent_yes_no.value == "Non [Hapana]" )
-{ tw.youth_data.current.last_name.value = "Unknown" ;}
-else { tw.youth_data.current.last_name.value = "Unknown" ;}</t>
+else if ( tw.youth_data.current.youth_consent_yes_no.value == ”Non [Hapana]” )
+{ tw.youth_data.current.last_name.value = ”Unknown” ;}
+else { tw.youth_data.current.last_name.value = ”Unknown” ;}</t>
   </si>
   <si>
     <t>var d = new Date(0) ;
-if (tw.youth_data.current.has_carte_delecteur_present_calculation.value == "True" )
+if (tw.youth_data.current.has_carte_delecteur_present_calculation.value == ”True” )
 { tw.youth_data.current.birthdate.value = tw.youth_data.current.carte_dob.value ; }
-else if (tw.youth_data.current.youth_carte_yes_no.value == "Oui, pas vu [Ndio, haionekane]" || tw.youth_data.current.youth_carte_yes_no.value == "Non [Hapana]" )
+else if (tw.youth_data.current.youth_carte_yes_no.value == ”Oui, pas vu [Ndio, haionekane]” || tw.youth_data.current.youth_carte_yes_no.value == ”Non [Hapana]” )
 { tw.youth_data.current.birthdate.value = tw.youth_data.current.dob_no_doc.value ; }
 else { tw.youth_data.current.birthdate.value = d ;}</t>
   </si>
   <si>
-    <t>tw.youth_data.current.survey_type.value = "Census2";</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.youth_consent_yes_no.value == "Non [Hapana]" ) { tw.youth_data.current.is_refusing.value = "True2" ; }
-else { tw.youth_data.current.is_refusing.value = "False2" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.youth_present_or_in_docs.value == "True2" || tw.youth_data.current.youth_consent_yes_no.value ==  "Non [Hapana]" || tw.youth_data.current.has_youths_carte.value == "Non, le jeune ne possède pas une carte d’electeur [Hapana, kijana hana kadi ya kura]" || tw.youth_data.current.youth_carte_yes_no.value == "Non [Hapana]" )
-{tw.youth_data.current.is_successful.value = "True2";}
-else if ( tw.youth_data.current.new_info_questionnaire.value == "Non [Hapana]" )
-{tw.youth_data.current.is_successful.value = "False2";}
-else {tw.youth_data.current.is_successful.value = "False2";}</t>
-  </si>
-  <si>
-    <t>if ( tw.youth_data.current.is_successful.value == "True2" ) 
-{ tw.youth_data.current.stage.value = "Census Complete2" ; } 
-else { tw.youth_data.current.stage.value = "Census2" ; }</t>
+    <t>tw.youth_data.current.survey_type.value = ”Census2”;</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.youth_consent_yes_no.value == ”Non [Hapana]” ) { tw.youth_data.current.is_refusing.value = ”True2” ; }
+else { tw.youth_data.current.is_refusing.value = ”False2” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.youth_present_or_in_docs.value == ”True2” || tw.youth_data.current.youth_consent_yes_no.value ==  ”Non [Hapana]” || tw.youth_data.current.has_youths_carte.value == ”Non, le jeune ne possède pas une carte d’electeur [Hapana, kijana hana kadi ya kura]” || tw.youth_data.current.youth_carte_yes_no.value == ”Non [Hapana]” )
+{tw.youth_data.current.is_successful.value = ”True2”;}
+else if ( tw.youth_data.current.new_info_questionnaire.value == ”Non [Hapana]” )
+{tw.youth_data.current.is_successful.value = ”False2”;}
+else {tw.youth_data.current.is_successful.value = ”False2”;}</t>
+  </si>
+  <si>
+    <t>if ( tw.youth_data.current.is_successful.value == ”True2” ) 
+{ tw.youth_data.current.stage.value = ”Census Complete2” ; } 
+else { tw.youth_data.current.stage.value = ”Census2” ; }</t>
   </si>
   <si>
     <t>tw.youth_data.current.device_id.value = tw.getIMEI();</t>
@@ -1590,54 +1590,54 @@
     <t>tw.youth_data.current.execution_date.value = new Date();</t>
   </si>
   <si>
-    <t>if ( tw.locating_the_household.needs_token_calculation.value == "True" &amp;amp;&amp;amp; tw.locating_the_household.abandoned_yes_no.value == "Non [Hapana]" )
-{ tw.calculating_relocation.needs_token_not_abandoned_calculation.value = "True" ; }
-else { tw.calculating_relocation.needs_token_not_abandoned_calculation.value = "False" ; }</t>
-  </si>
-  <si>
-    <t>var showQuestion = "False" ; 
+    <t>if ( tw.locating_the_household.needs_token_calculation.value == ”True” &amp;amp;&amp;amp; tw.locating_the_household.abandoned_yes_no.value == ”Non [Hapana]” )
+{ tw.calculating_relocation.needs_token_not_abandoned_calculation.value = ”True” ; }
+else { tw.calculating_relocation.needs_token_not_abandoned_calculation.value = ”False” ; }</t>
+  </si>
+  <si>
+    <t>var showQuestion = ”False” ; 
 if ( tw.youth_data !== null )
 { for (var i = 0; i &amp;lt; tw.youth_data.length ; i++) {
     var youth_data = tw.youth_data[i];
     if (youth_data.is_successful.value == ’False2’ ) {
-        showQuestion = "True" ;
+        showQuestion = ”True” ;
     }
 } }
 tw.calculating_relocation.should_relocating_show.value = showQuestion ;</t>
   </si>
   <si>
-    <t>if ( ( tw.drill_down.is_available_pulled_down.value == null || tw.drill_down.is_18_available_pulled_down.value == null ) &amp;amp;&amp;amp; tw.locating_the_household.available_yes_no.value == "Oui [Ndiyo]" )
-{ tw.calculating_relocation.should_s6_show.value = "True" ; }
-else if ( tw.drill_down.is_nah_revisit_calculation.value == "True2" &amp;amp;&amp;amp; tw.locating_the_household.available_yes_no.value == "Oui [Ndiyo]" )
- { tw.calculating_relocation.should_s6_show.value = "True" ; } 
-else if ( tw.locating_the_household.abandoned_yes_no.value == "Non [Hapana]" )
- { tw.calculating_relocation.should_s6_show.value = "True" ; } 
-else { tw.calculating_relocation.should_s6_show.value = "False" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.participation_and_consent.above_18_other_later_yes_no.value == "Non [Hapana]" || tw.participation_and_consent.refusing_yes_no.value == "Non [Hapana]" || tw.hh_presence.terminate_yes_no.value == "Non/Je ne sais pas [Hapana/Sijuwe]" ) 
-{ tw.calculating_relocation.hide_fraud_detection.value = "True" ; }
-else { tw.calculating_relocation.hide_fraud_detection.value = "False" ; }</t>
-  </si>
-  <si>
-    <t>var noReasonProvided = tw.relocating.test_2.value.contains("Je ne sais pas [Sijui]"); 
-var otherReasonProvided = tw.relocating.test_2.value.contains("Au boulot [Kazini]") || tw.relocating.test_2.value.contains("L\’école [Shuleni]") || tw.relocating.test_2.value.contains("Vient de sortir [Imetoka tu]") || tw.relocating.test_2.value.contains("En dehors de la ville [Inje ya muji]") || tw.relocating.test_2.value.contains("Autre [Yengine]" ) ;
+    <t>if ( ( tw.drill_down.is_available_pulled_down.value == null || tw.drill_down.is_18_available_pulled_down.value == null ) &amp;amp;&amp;amp; tw.locating_the_household.available_yes_no.value == ”Oui [Ndiyo]” )
+{ tw.calculating_relocation.should_s6_show.value = ”True” ; }
+else if ( tw.drill_down.is_nah_revisit_calculation.value == ”True2” &amp;amp;&amp;amp; tw.locating_the_household.available_yes_no.value == ”Oui [Ndiyo]” )
+ { tw.calculating_relocation.should_s6_show.value = ”True” ; } 
+else if ( tw.locating_the_household.abandoned_yes_no.value == ”Non [Hapana]” )
+ { tw.calculating_relocation.should_s6_show.value = ”True” ; } 
+else { tw.calculating_relocation.should_s6_show.value = ”False” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.participation_and_consent.above_18_other_later_yes_no.value == ”Non [Hapana]” || tw.participation_and_consent.refusing_yes_no.value == ”Non [Hapana]” || tw.hh_presence.terminate_yes_no.value == ”Non/Je ne sais pas [Hapana/Sijuwe]” ) 
+{ tw.calculating_relocation.hide_fraud_detection.value = ”True” ; }
+else { tw.calculating_relocation.hide_fraud_detection.value = ”False” ; }</t>
+  </si>
+  <si>
+    <t>var noReasonProvided = tw.relocating.test_2.value.contains(”Je ne sais pas [Sijui]”); 
+var otherReasonProvided = tw.relocating.test_2.value.contains(”Au boulot [Kazini]”) || tw.relocating.test_2.value.contains(”L\’école [Shuleni]”) || tw.relocating.test_2.value.contains(”Vient de sortir [Imetoka tu]”) || tw.relocating.test_2.value.contains(”En dehors de la ville [Inje ya muji]”) || tw.relocating.test_2.value.contains(”Autre [Yengine]” ) ;
 if (noReasonProvided &amp;amp;&amp;amp; otherReasonProvided) 
-{ throw "Vous avez sélectionné la réponse Je ne sais pas et une autre reponse! [Ulichagua Sijui na jibu yengine!]"; }</t>
-  </si>
-  <si>
-    <t>var noReasonProvided = tw.relocating.youth_revisit_time_updated.value.contains("Je ne sais pas [Sijui]"); 
-var otherReasonProvided = tw.relocating.youth_revisit_time_updated.value.contains("Matin en semaine [Asubuyi siku la juma]") || tw.relocating.youth_revisit_time_updated.value.contains("Après-midi en semaine [Kisha mchana siku la juma]") || tw.relocating.youth_revisit_time_updated.value.contains("Samedi matin [Jumamosi asubuyi]") || tw.relocating.youth_revisit_time_updated.value.contains("Samedi après-midi [Jumamosi kisha mchana]") || tw.relocating.youth_revisit_time_updated.value.contains("Dimanche matin [Jumapili asubuyi]") || tw.relocating.youth_revisit_time_updated.value.contains("Dimanche après-midi [Jumapili kisha mchana]") || tw.relocating.youth_revisit_time_updated.value.contains("A partir d’une date précise (sélectionner dans la question suivante) [Kwa tarehe ijulikanayo (changua ndani ya swali ifuuatao)]") ; 
-if (noReasonProvided &amp;amp;&amp;amp; otherReasonProvided) { throw "Vous avez sélectionné la réponse Je ne sais pas et une autre reponse! [Ulichagua Sijui na jibu yengine!]"; }</t>
-  </si>
-  <si>
-    <t>var dt = tw.participation_and_consent.revisit_when.value ; if (dt.getFullYear() &amp;lt;=2018) {throw "Le moment de la visite suivante ne peut pas être dans le passé! [Wakati wa kurudi hauwezi kuwa kwa muda iliyo pita!]" ;} else if (dt.getFullYear() == 2019 &amp;amp;&amp;amp; dt.getMonth() &amp;lt;7) {throw "Le moment de la visite suivante ne peut pas être dans le passé! [Wakati wa kurudi hauwezi kuwa kwa muda iliyo pita!]" ;}</t>
-  </si>
-  <si>
-    <t>if ( tw.relocating_hh.read.value == "Non [Hapana]" ) { tw.relocating_hh.should_flyer_token_show.value = "True" ; }
-else if ( tw.participation_and_consent.family_or_renter_calc.value == "False" || tw.participation_and_consent.above_18_yes_no.value == "Personne n’a 18 ou plus [Hakuna mtu aliye na miaka 18+]" || tw.participation_and_consent.refusing_yes_no.value == "Non [Hapana]" || tw.hh_presence.terminate_yes_no.value == "Non/Je ne sais pas [Hapana/Sijuwe]" || tw.calculating_relocation.needs_token_not_abandoned_calculation.value == "True" ) 
- { tw.relocating_hh.should_flyer_token_show.value = "True" ; }
-else  { tw.relocating_hh.should_flyer_token_show.value = "False" ; }</t>
+{ throw ”Vous avez sélectionné la réponse Je ne sais pas et une autre reponse! [Ulichagua Sijui na jibu yengine!]”; }</t>
+  </si>
+  <si>
+    <t>var noReasonProvided = tw.relocating.youth_revisit_time_updated.value.contains(”Je ne sais pas [Sijui]”); 
+var otherReasonProvided = tw.relocating.youth_revisit_time_updated.value.contains(”Matin en semaine [Asubuyi siku la juma]”) || tw.relocating.youth_revisit_time_updated.value.contains(”Après-midi en semaine [Kisha mchana siku la juma]”) || tw.relocating.youth_revisit_time_updated.value.contains(”Samedi matin [Jumamosi asubuyi]”) || tw.relocating.youth_revisit_time_updated.value.contains(”Samedi après-midi [Jumamosi kisha mchana]”) || tw.relocating.youth_revisit_time_updated.value.contains(”Dimanche matin [Jumapili asubuyi]”) || tw.relocating.youth_revisit_time_updated.value.contains(”Dimanche après-midi [Jumapili kisha mchana]”) || tw.relocating.youth_revisit_time_updated.value.contains(”A partir d’une date précise (sélectionner dans la question suivante) [Kwa tarehe ijulikanayo (changua ndani ya swali ifuuatao)]”) ; 
+if (noReasonProvided &amp;amp;&amp;amp; otherReasonProvided) { throw ”Vous avez sélectionné la réponse Je ne sais pas et une autre reponse! [Ulichagua Sijui na jibu yengine!]”; }</t>
+  </si>
+  <si>
+    <t>var dt = tw.participation_and_consent.revisit_when.value ; if (dt.getFullYear() &amp;lt;=2018) {throw ”Le moment de la visite suivante ne peut pas être dans le passé! [Wakati wa kurudi hauwezi kuwa kwa muda iliyo pita!]” ;} else if (dt.getFullYear() == 2019 &amp;amp;&amp;amp; dt.getMonth() &amp;lt;7) {throw ”Le moment de la visite suivante ne peut pas être dans le passé! [Wakati wa kurudi hauwezi kuwa kwa muda iliyo pita!]” ;}</t>
+  </si>
+  <si>
+    <t>if ( tw.relocating_hh.read.value == ”Non [Hapana]” ) { tw.relocating_hh.should_flyer_token_show.value = ”True” ; }
+else if ( tw.participation_and_consent.family_or_renter_calc.value == ”False” || tw.participation_and_consent.above_18_yes_no.value == ”Personne n’a 18 ou plus [Hakuna mtu aliye na miaka 18+]” || tw.participation_and_consent.refusing_yes_no.value == ”Non [Hapana]” || tw.hh_presence.terminate_yes_no.value == ”Non/Je ne sais pas [Hapana/Sijuwe]” || tw.calculating_relocation.needs_token_not_abandoned_calculation.value == ”True” ) 
+ { tw.relocating_hh.should_flyer_token_show.value = ”True” ; }
+else  { tw.relocating_hh.should_flyer_token_show.value = ”False” ; }</t>
   </si>
   <si>
     <t>tw.relocating_hh.token.value = tw.locating_the_household.token_number.value ;</t>
@@ -1646,79 +1646,79 @@
     <t>tw.relocating_hh.token_flyer_3.value = tw.locating_the_household.token_number.value ;</t>
   </si>
   <si>
-    <t>if (tw.relocating_hh.token_confirm.value != "Oui [Ndiyo]") {throw "Chaque ménage recensé doit recevoir un numéro d’identification. [Kila nyumba iliyo fatwa anapashwa pokean nambari ya ishara.]" ;}</t>
-  </si>
-  <si>
-    <t>if ( tw.participation_and_consent.fo_upfront_security.value == "Non [Hapana]" &amp;amp;&amp;amp; tw.participation_and_consent.fo_upfront_leave_yes_no.value == "Oui [Ndiyo]" ) { tw.fraud_detection.feels_unsafe_end_early.value = "True" ; }
-else { tw.fraud_detection.feels_unsafe_end_early.value = "False" ; }</t>
+    <t>if (tw.relocating_hh.token_confirm.value != ”Oui [Ndiyo]”) {throw ”Chaque ménage recensé doit recevoir un numéro d’identification. [Kila nyumba iliyo fatwa anapashwa pokean nambari ya ishara.]” ;}</t>
+  </si>
+  <si>
+    <t>if ( tw.participation_and_consent.fo_upfront_security.value == ”Non [Hapana]” &amp;amp;&amp;amp; tw.participation_and_consent.fo_upfront_leave_yes_no.value == ”Oui [Ndiyo]” ) { tw.fraud_detection.feels_unsafe_end_early.value = ”True” ; }
+else { tw.fraud_detection.feels_unsafe_end_early.value = ”False” ; }</t>
   </si>
   <si>
     <t>var str = tw.fraud_detection.lie_descript.value ; 
-var length = str.length ; if (length &amp;lt; 25) {throw "Minimum 25 caractères. Veuillez entrer plus d’informations pour cette description. [Kiwango cha chini cha herufi 25. Tafadhali ingiza zaidi kwa maelezo haya.]" ;}</t>
+var length = str.length ; if (length &amp;lt; 25) {throw ”Minimum 25 caractères. Veuillez entrer plus d’informations pour cette description. [Kiwango cha chini cha herufi 25. Tafadhali ingiza zaidi kwa maelezo haya.]” ;}</t>
   </si>
   <si>
     <t>var str = tw.fraud_detection.security_descript.value ; 
 var length = str.length ; 
-if (length &amp;lt; 25) {throw "Minimum 25 caractères. Veuillez entrer plus d’informations pour cette description. [Kiwango cha chini cha herufi 25. Tafadhali ingiza zaidi kwa maelezo haya.]" ;}</t>
-  </si>
-  <si>
-    <t>if ( tw.drill_down.is_youth_yn_filled_pulled_down.value == "True2" ) 
-{ tw.conclusion.is_household_description_filled.value = "True2" ; }
-else if ( tw.hh_presence.youths_yes_no.value == "Oui, l’enquêté confirme qu’il y a des jeunes dans ce ménage (peut inclure l’enquêté) [Ndio, mhojiwa anakubali kwamba kuna vijana katika nyumba hii (inaweza kujumuisha mhojiwa)]" || tw.hh_presence.youths_yes_no.value == "Non, l’enquêté confirme qu’il n’y a pas de jeunes dans ce ménage [Apana, mhojiwa anakubali kuwa hakuna vijana katika nyumba hii]" || tw.hh_presence.youths_yes_no.value == "Personne ici présent sait [Hakuna yeyote hapa anajua]" )
-{ tw.conclusion.is_household_description_filled.value = "True2" ; }
-else { tw.conclusion.is_household_description_filled.value = "False2" ; }</t>
-  </si>
-  <si>
-    <t>if ( ( tw.participation_and_consent.above_18_other_later_yes_no.value == "Oui [Ndiyo]" || tw.participation_and_consent.refusing_household_position.value == "Non [Hapana]" || tw.locating_the_household.abandoned_yes_no.value == "Non [Hapana]" || tw.participation_and_consent.fo_upfront_leave_yes_no.value == "Non [Hapana]" || tw.hh_presence.youths_yes_no.value == "Oui, l’enquêté confirme qu’il y a des jeunes dans ce ménage (peut inclure l’enquêté) [Ndio, mhojiwa anakubali kwamba kuna vijana katika nyumba hii (inaweza kujumuisha mhojiwa)]" ) &amp;amp;&amp;amp; ( tw.drill_down.house_description_pulled_down.value == null || tw.drill_down.house_description_pulled_down.value == ’null’ || tw.drill_down.house_description_pulled_down.value == " " ) )
-{ tw.conclusion.should_conc_be_limited.value = "True"; }
-else {tw.conclusion.should_conc_be_limited.value = "False";}</t>
-  </si>
-  <si>
-    <t>if ( ( tw.participation_and_consent.above_18_other_later_yes_no.value == "Oui [Ndiyo]" || tw.participation_and_consent.refusing_household_position.value == "Non [Hapana]" || tw.locating_the_household.abandoned_yes_no.value == "Non [Hapana]" || tw.participation_and_consent.fo_upfront_leave_yes_no.value == "Oui [Ndiyo]" ) &amp;amp;&amp;amp; ( tw.drill_down.mairie_number_pulled_down.value == null || tw.drill_down.mairie_number_pulled_down.value == ’null’ || tw.drill_down.mairie_number_pulled_down.value == " " ) )
-{ tw.conclusion.early_mairie_number_show_calculation.value = "True" ; }
-else { tw.conclusion.early_mairie_number_show_calculation.value = "False" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.conclusion.early_mairie_number_show_calculation.value == "False" &amp;amp;&amp;amp; tw.hh_presence.youths_yes_no.value == "Oui, l’enquêté confirme qu’il y a des jeunes dans ce ménage (peut inclure l’enquêté) [Ndio, mhojiwa anakubali kwamba kuna vijana katika nyumba hii (inaweza kujumuisha mhojiwa)]" &amp;amp;&amp;amp; ( tw.drill_down.mairie_number_pulled_down.value == null || tw.drill_down.mairie_number_pulled_down.value == ’null’ || tw.drill_down.mairie_number_pulled_down.value == " " ) )
-{ tw.conclusion.should_mairie_number_show_calculation.value = "True" ; }
-else { tw.conclusion.should_mairie_number_show_calculation.value = "False" ; }</t>
+if (length &amp;lt; 25) {throw ”Minimum 25 caractères. Veuillez entrer plus d’informations pour cette description. [Kiwango cha chini cha herufi 25. Tafadhali ingiza zaidi kwa maelezo haya.]” ;}</t>
+  </si>
+  <si>
+    <t>if ( tw.drill_down.is_youth_yn_filled_pulled_down.value == ”True2” ) 
+{ tw.conclusion.is_household_description_filled.value = ”True2” ; }
+else if ( tw.hh_presence.youths_yes_no.value == ”Oui, l’enquêté confirme qu’il y a des jeunes dans ce ménage (peut inclure l’enquêté) [Ndio, mhojiwa anakubali kwamba kuna vijana katika nyumba hii (inaweza kujumuisha mhojiwa)]” || tw.hh_presence.youths_yes_no.value == ”Non, l’enquêté confirme qu’il n’y a pas de jeunes dans ce ménage [Apana, mhojiwa anakubali kuwa hakuna vijana katika nyumba hii]” || tw.hh_presence.youths_yes_no.value == ”Personne ici présent sait [Hakuna yeyote hapa anajua]” )
+{ tw.conclusion.is_household_description_filled.value = ”True2” ; }
+else { tw.conclusion.is_household_description_filled.value = ”False2” ; }</t>
+  </si>
+  <si>
+    <t>if ( ( tw.participation_and_consent.above_18_other_later_yes_no.value == ”Oui [Ndiyo]” || tw.participation_and_consent.refusing_household_position.value == ”Non [Hapana]” || tw.locating_the_household.abandoned_yes_no.value == ”Non [Hapana]” || tw.participation_and_consent.fo_upfront_leave_yes_no.value == ”Non [Hapana]” || tw.hh_presence.youths_yes_no.value == ”Oui, l’enquêté confirme qu’il y a des jeunes dans ce ménage (peut inclure l’enquêté) [Ndio, mhojiwa anakubali kwamba kuna vijana katika nyumba hii (inaweza kujumuisha mhojiwa)]” ) &amp;amp;&amp;amp; ( tw.drill_down.house_description_pulled_down.value == null || tw.drill_down.house_description_pulled_down.value == ’null’ || tw.drill_down.house_description_pulled_down.value == ” ” ) )
+{ tw.conclusion.should_conc_be_limited.value = ”True”; }
+else {tw.conclusion.should_conc_be_limited.value = ”False”;}</t>
+  </si>
+  <si>
+    <t>if ( ( tw.participation_and_consent.above_18_other_later_yes_no.value == ”Oui [Ndiyo]” || tw.participation_and_consent.refusing_household_position.value == ”Non [Hapana]” || tw.locating_the_household.abandoned_yes_no.value == ”Non [Hapana]” || tw.participation_and_consent.fo_upfront_leave_yes_no.value == ”Oui [Ndiyo]” ) &amp;amp;&amp;amp; ( tw.drill_down.mairie_number_pulled_down.value == null || tw.drill_down.mairie_number_pulled_down.value == ’null’ || tw.drill_down.mairie_number_pulled_down.value == ” ” ) )
+{ tw.conclusion.early_mairie_number_show_calculation.value = ”True” ; }
+else { tw.conclusion.early_mairie_number_show_calculation.value = ”False” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.conclusion.early_mairie_number_show_calculation.value == ”False” &amp;amp;&amp;amp; tw.hh_presence.youths_yes_no.value == ”Oui, l’enquêté confirme qu’il y a des jeunes dans ce ménage (peut inclure l’enquêté) [Ndio, mhojiwa anakubali kwamba kuna vijana katika nyumba hii (inaweza kujumuisha mhojiwa)]” &amp;amp;&amp;amp; ( tw.drill_down.mairie_number_pulled_down.value == null || tw.drill_down.mairie_number_pulled_down.value == ’null’ || tw.drill_down.mairie_number_pulled_down.value == ” ” ) )
+{ tw.conclusion.should_mairie_number_show_calculation.value = ”True” ; }
+else { tw.conclusion.should_mairie_number_show_calculation.value = ”False” ; }</t>
   </si>
   <si>
     <t>var mairieRegex = /^[0-9]{2,3}[A-Z a-z]{1}$/ ;
 var mairienumRegex = /^[0-9]{3}$/ ;
 if (!mairieRegex.test(tw.conclusion.mairie_num.value) &amp;amp;&amp;amp; !mairienumRegex(tw.conclusion.mairie_num.value))
-{throw "Le format correct d’un numéro de mairie est de 2-3 chiffres suivis d’une lettre OU de 3 chiffres. Exemples: 12A ou 123A OU 123. [Fomati kweli ya namba ya meya iko na namba 2-3 ziki chindikizwa na erufi ama na namba 3. Mufano: 12A ama 123A ama 123A ama 123.]" ;}</t>
+{throw ”Le format correct d’un numéro de mairie est de 2-3 chiffres suivis d’une lettre OU de 3 chiffres. Exemples: 12A ou 123A OU 123. [Fomati kweli ya namba ya meya iko na namba 2-3 ziki chindikizwa na erufi ama na namba 3. Mufano: 12A ama 123A ama 123A ama 123.]” ;}</t>
   </si>
   <si>
     <t>if(tw.conclusion.mairie_num_reentry.value != tw.conclusion.mairie_num.value) 
-{throw "Ce numéro de mairie ne correspond pas à celui du numero de la mairie que vous venez d’entrer! [Nambari hii ya ukumbi wa jiji hailingani na nambari ya ukumbi wa jiji iliyoingia tu!]" ; }</t>
+{throw ”Ce numéro de mairie ne correspond pas à celui du numero de la mairie que vous venez d’entrer! [Nambari hii ya ukumbi wa jiji hailingani na nambari ya ukumbi wa jiji iliyoingia tu!]” ; }</t>
   </si>
   <si>
     <t>if(tw.conclusion.other_num_ind_reentry.value != tw.conclusion.other_num_ind_entry.value) 
-{throw "Ce numéro ne correspond pas à celui que vous venez d’entrer! [Nambari hii hailingani na nambari uliyoingia hivi karibuni!]" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.conclusion.leave_early_mairie_yes_no.value == "Oui [Ndiyo]" || tw.conclusion.mairie_yes_no.value == "Oui [Ndiyo]" )
-{ tw.conclusion.does_hh_have_mairie.value = "True" ; }
-else { tw.conclusion.does_hh_have_mairie.value = "False" ; }</t>
-  </si>
-  <si>
-    <t>if ( tw.conclusion.leave_early_other_num_yes_no.value == "Oui [Ndiyo]" || tw.conclusion.dif_num_yes_no.value == "Oui [Ndiyo]" )
-{ tw.conclusion.does_hh_have_other_num.value = "True" ; }
-else { tw.conclusion.does_hh_have_other_num.value = "False" ; }</t>
+{throw ”Ce numéro ne correspond pas à celui que vous venez d’entrer! [Nambari hii hailingani na nambari uliyoingia hivi karibuni!]” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.conclusion.leave_early_mairie_yes_no.value == ”Oui [Ndiyo]” || tw.conclusion.mairie_yes_no.value == ”Oui [Ndiyo]” )
+{ tw.conclusion.does_hh_have_mairie.value = ”True” ; }
+else { tw.conclusion.does_hh_have_mairie.value = ”False” ; }</t>
+  </si>
+  <si>
+    <t>if ( tw.conclusion.leave_early_other_num_yes_no.value == ”Oui [Ndiyo]” || tw.conclusion.dif_num_yes_no.value == ”Oui [Ndiyo]” )
+{ tw.conclusion.does_hh_have_other_num.value = ”True” ; }
+else { tw.conclusion.does_hh_have_other_num.value = ”False” ; }</t>
   </si>
   <si>
     <t>var str = tw.conclusion.house_description.value ;
 var length = str.length ;
-if (length &amp;lt; 30) {throw "Minimum 30 caractères. Veuillez entrer plus d’informations pour cette description. [Kiwango cha chini cha herufi/hesabu 30. Tafadhali ingiza zaidi kwa maelezo haya.]" ;}
-else if (length &amp;gt; 250) {throw "Maximum 250 caractères. Veuillez entrer moins d’informations pour cette description. [Kiwango cha chini cha herufi/hesabu 250. Tafadhali ingiza maelezo machache.]" ;}
+if (length &amp;lt; 30) {throw ”Minimum 30 caractères. Veuillez entrer plus d’informations pour cette description. [Kiwango cha chini cha herufi/hesabu 30. Tafadhali ingiza zaidi kwa maelezo haya.]” ;}
+else if (length &amp;gt; 250) {throw ”Maximum 250 caractères. Veuillez entrer moins d’informations pour cette description. [Kiwango cha chini cha herufi/hesabu 250. Tafadhali ingiza maelezo machache.]” ;}
 if ( tw.drill_down.house_description_pulled_down.value !== null )
 { tw.conclusion.house_description.value = tw.drill_down.house_description_pulled_down.value ; }</t>
   </si>
   <si>
     <t>var current = parseInt( tw.drill_down.household_survey_counter_pulled_down.value ) ; 
 var updated = current + 1 ; 
-if (tw.drill_down.is_first_visit_calculation.value == "True2") { tw.conclusion.household_survey_counter_1.value = "1" ; }
+if (tw.drill_down.is_first_visit_calculation.value == ”True2”) { tw.conclusion.household_survey_counter_1.value = ”1” ; }
 else { tw.conclusion.household_survey_counter_1.value = updated.toString() ; }</t>
   </si>
   <si>
@@ -1736,8 +1736,8 @@
   <si>
     <t>var firstvisit = tw.drill_down.is_first_visit_nah_pulled_down.value ;
 if ( firstvisit !== null ) { tw.conclusion.is_first_visit_nah.value = firstvisit ; }
-else if ( tw.drill_down.is_first_visit_calculation.value == "True2" &amp;amp;&amp;amp; ( tw.locating_the_household.abandoned_yes_no.value == "Non [Hapana]" || tw.participation_and_consent.above_18_yes_no.value == "Personne n’a 18 ou plus [Hakuna mtu aliye na miaka 18+]" || tw.participation_and_consent.refusing_household_position.value == "Non [Hapana]" ) ) { tw.conclusion.is_first_visit_nah.value = "True2" ; }
-else { tw.conclusion.is_first_visit_nah.value = "False2" ; }</t>
+else if ( tw.drill_down.is_first_visit_calculation.value == ”True2” &amp;amp;&amp;amp; ( tw.locating_the_household.abandoned_yes_no.value == ”Non [Hapana]” || tw.participation_and_consent.above_18_yes_no.value == ”Personne n’a 18 ou plus [Hakuna mtu aliye na miaka 18+]” || tw.participation_and_consent.refusing_household_position.value == ”Non [Hapana]” ) ) { tw.conclusion.is_first_visit_nah.value = ”True2” ; }
+else { tw.conclusion.is_first_visit_nah.value = ”False2” ; }</t>
   </si>
   <si>
     <t>Calculation</t>
@@ -1793,7 +1793,7 @@
 Ninakiri kuwa nimeeleweshwa kikamilifu na nimeamua kutopokea ushauri wa washauri (wenye siasa) katika suala hili. Ninaelewa kuwa nina haki ya kujua nani data hii imeshirikiwa kwake / ao kuomba kwamba habari juu yangu ibadilishwe ao kuvutwa, ingawa hii inaweza kutosha ushiriki wangu katika mpango unaoweza kutokea baadaye.]</t>
   </si>
   <si>
-    <t>var indInfoString = "Le nom de ce jeune est inconnu. Verifiez si vous n’êtes pas en train de prendre des informations sur des jeunes dont les noms sont déjà connus. [Jina la huyu kijana haijulikane. Angaliya tena listi ili usi chukue habari juu ya kijana ambaye anajulikana tayari]." ;
+    <t>var indInfoString = ”Le nom de ce jeune est inconnu. Verifiez si vous n’êtes pas en train de prendre des informations sur des jeunes dont les noms sont déjà connus. [Jina la huyu kijana haijulikane. Angaliya tena listi ili usi chukue habari juu ya kijana ambaye anajulikana tayari].” ;
 tw.youth_data.current.youth_name_is_unknown.value = indInfoString ;</t>
   </si>
   <si>

</xml_diff>